<commit_message>
Decimal outputs to BigQuery as numeric
</commit_message>
<xml_diff>
--- a/projects/gain_tracker/tests/positions_sample.xlsx
+++ b/projects/gain_tracker/tests/positions_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mirth\src\trader_buddy\projects\gain_tracker\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2862FFCA-3C28-4F5A-BA7B-24FD66845C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EB249E-1BB4-4B9C-927C-A12EB7CEDBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40230" yWindow="3970" windowWidth="22620" windowHeight="16210" xr2:uid="{728E0C82-911A-4918-A535-4E940BC738FC}"/>
   </bookViews>
@@ -558,7 +558,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
test asset for pulling historic prices for benchmark using yfinance
</commit_message>
<xml_diff>
--- a/projects/gain_tracker/tests/positions_sample.xlsx
+++ b/projects/gain_tracker/tests/positions_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mirth\src\trader_buddy\projects\gain_tracker\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EB249E-1BB4-4B9C-927C-A12EB7CEDBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C46F5A-589E-476D-BECD-F3F156BFBE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40230" yWindow="3970" windowWidth="22620" windowHeight="16210" xr2:uid="{728E0C82-911A-4918-A535-4E940BC738FC}"/>
   </bookViews>
@@ -558,7 +558,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>